<commit_message>
Commit-8-Running Login Test for Invalid data from excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/OpenEmrData.xlsx
+++ b/src/test/resources/testdata/OpenEmrData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scientificgames-my.sharepoint.com/personal/rachana_nagaraja_sgdigital_com/Documents/Automation/Excel sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scientificgames-my.sharepoint.com/personal/rachana_nagaraja_sgdigital_com/Documents/Automation/java_eclipse_workspace/OpenEmrApplication1/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{60F4D58C-636B-4917-865E-CB8F93C7C059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBFED471-B09C-4B4C-A8A6-99D7D2EB245A}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{60F4D58C-636B-4917-865E-CB8F93C7C059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B269D1B-AF43-48F2-A430-5D1DAAB81D90}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DDD1171C-8EB4-4633-9875-0A59037B1795}"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7360" xr2:uid="{DDD1171C-8EB4-4633-9875-0A59037B1795}"/>
   </bookViews>
   <sheets>
     <sheet name="inValidCrendentialTest" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>English (Indian)</t>
   </si>
   <si>
-    <t>Invalid Username and Password</t>
-  </si>
-  <si>
     <t>john</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>Dutch</t>
+  </si>
+  <si>
+    <t>Invalid username or password</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -457,21 +457,21 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit9-To push the code
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/OpenEmrData.xlsx
+++ b/src/test/resources/testdata/OpenEmrData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scientificgames-my.sharepoint.com/personal/rachana_nagaraja_sgdigital_com/Documents/Automation/java_eclipse_workspace/OpenEmrApplication1/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{60F4D58C-636B-4917-865E-CB8F93C7C059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B93CF5BE-81B7-4BC5-B9CC-85757A4DC729}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{60F4D58C-636B-4917-865E-CB8F93C7C059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AC1E768-2AA9-449B-AB5C-8E736DC823A5}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7360" xr2:uid="{DDD1171C-8EB4-4633-9875-0A59037B1795}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Username</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Test123</t>
-  </si>
-  <si>
-    <t>Invalid username and password</t>
   </si>
 </sst>
 </file>
@@ -430,7 +427,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,7 +491,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>